<commit_message>
feat：update dragongirl icon change
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/BagItem_背包物品表.xlsx
+++ b/dragon-verse/Excels/BagItem_背包物品表.xlsx
@@ -499,7 +499,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -556,10 +556,6 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -573,10 +569,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -791,10 +783,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S2000"/>
+  <dimension ref="A1:N2000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1136,7 +1128,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B12,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="9" t="s">
         <v>34</v>
       </c>
       <c r="E12" s="7" t="str">
@@ -1167,7 +1159,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B13,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="9" t="s">
         <v>36</v>
       </c>
       <c r="E13" s="7" t="str">
@@ -1232,7 +1224,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B15,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="9" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="7" t="str">
@@ -1265,7 +1257,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B16,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="9" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="7" t="str">
@@ -1298,7 +1290,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B17,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="9" t="s">
         <v>44</v>
       </c>
       <c r="E17" s="7" t="str">
@@ -1331,7 +1323,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B18,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="9" t="s">
         <v>46</v>
       </c>
       <c r="E18" s="7" t="str">
@@ -1364,7 +1356,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B19,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="9" t="s">
         <v>48</v>
       </c>
       <c r="E19" s="7" t="str">
@@ -1430,7 +1422,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B21,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="9" t="s">
         <v>52</v>
       </c>
       <c r="E21" s="7" t="str">
@@ -1490,7 +1482,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B23,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="9" t="s">
         <v>56</v>
       </c>
       <c r="E23" s="7" t="str">
@@ -1550,7 +1542,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B25,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="9" t="s">
         <v>60</v>
       </c>
       <c r="E25" s="7" t="str">
@@ -1580,7 +1572,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B26,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="9" t="s">
         <v>62</v>
       </c>
       <c r="E26" s="7" t="str">
@@ -1610,14 +1602,14 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B27,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="9" t="s">
         <v>64</v>
       </c>
       <c r="E27" s="7" t="str">
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($D27,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="F27" s="15" t="n">
+      <c r="F27" s="14" t="n">
         <v>326270</v>
       </c>
       <c r="G27" s="2" t="n">
@@ -1640,7 +1632,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B28,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D28" s="14" t="s">
+      <c r="D28" s="9" t="s">
         <v>66</v>
       </c>
       <c r="E28" s="7" t="str">
@@ -1670,7 +1662,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B29,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="9" t="s">
         <v>68</v>
       </c>
       <c r="E29" s="2" t="str">
@@ -1700,7 +1692,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B30,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="15" t="s">
         <v>70</v>
       </c>
       <c r="E30" s="2" t="str">
@@ -1730,7 +1722,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B31,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="15" t="s">
         <v>72</v>
       </c>
       <c r="E31" s="2" t="str">
@@ -1760,7 +1752,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B32,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="16" t="s">
         <v>74</v>
       </c>
       <c r="E32" s="13" t="str">
@@ -1790,7 +1782,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B33,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="16" t="s">
         <v>76</v>
       </c>
       <c r="E33" s="13" t="str">
@@ -1820,7 +1812,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B34,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="15" t="s">
         <v>78</v>
       </c>
       <c r="E34" s="2" t="str">
@@ -1850,7 +1842,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B35,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="15" t="s">
         <v>80</v>
       </c>
       <c r="E35" s="2" t="str">
@@ -1880,7 +1872,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B36,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="16" t="s">
         <v>82</v>
       </c>
       <c r="E36" s="13" t="str">
@@ -1909,7 +1901,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B37,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="15" t="s">
         <v>84</v>
       </c>
       <c r="E37" s="2" t="str">
@@ -1938,7 +1930,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B38,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="15" t="s">
         <v>86</v>
       </c>
       <c r="E38" s="2" t="str">
@@ -1967,7 +1959,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B39,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="15" t="s">
         <v>88</v>
       </c>
       <c r="E39" s="2" t="str">
@@ -1996,7 +1988,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B40,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="15" t="s">
         <v>90</v>
       </c>
       <c r="E40" s="2" t="str">
@@ -2025,7 +2017,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B41,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="15" t="s">
         <v>92</v>
       </c>
       <c r="E41" s="2" t="str">
@@ -2054,7 +2046,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B42,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="15" t="s">
         <v>94</v>
       </c>
       <c r="E42" s="2" t="str">
@@ -2083,7 +2075,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B43,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D43" s="15" t="s">
         <v>96</v>
       </c>
       <c r="E43" s="2" t="str">
@@ -2112,7 +2104,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B44,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="15" t="s">
         <v>98</v>
       </c>
       <c r="E44" s="2" t="str">
@@ -2141,7 +2133,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B45,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="D45" s="15" t="s">
         <v>100</v>
       </c>
       <c r="E45" s="2" t="str">
@@ -2169,7 +2161,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B46,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="D46" s="15" t="s">
         <v>102</v>
       </c>
       <c r="E46" s="2" t="str">
@@ -2197,7 +2189,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B47,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="D47" s="15" t="s">
         <v>104</v>
       </c>
       <c r="E47" s="2" t="str">
@@ -2225,7 +2217,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B48,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="15" t="s">
         <v>106</v>
       </c>
       <c r="E48" s="2" t="str">
@@ -2242,7 +2234,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="13" t="n">
         <v>44</v>
       </c>
@@ -2253,7 +2245,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B49,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D49" s="17" t="s">
+      <c r="D49" s="16" t="s">
         <v>108</v>
       </c>
       <c r="E49" s="13" t="str">
@@ -2261,7 +2253,7 @@
         <v/>
       </c>
       <c r="F49" s="13" t="n">
-        <v>381553</v>
+        <v>386905</v>
       </c>
       <c r="G49" s="13" t="n">
         <v>1</v>
@@ -2269,19 +2261,8 @@
       <c r="H49" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="I49" s="18"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18"/>
-      <c r="L49" s="18"/>
-      <c r="M49" s="18"/>
-      <c r="N49" s="18"/>
-      <c r="O49" s="18"/>
-      <c r="P49" s="18"/>
-      <c r="Q49" s="18"/>
-      <c r="R49" s="18"/>
-      <c r="S49" s="18"/>
-    </row>
-    <row r="50" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="50" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="13" t="n">
         <v>45</v>
       </c>
@@ -2292,7 +2273,7 @@
         <f aca="true">IFERROR(INDEX(OFFSET([1]Sheet1!$D$1,0,0,MaxCount),MATCH($B50,OFFSET([1]Sheet1!$B$1,0,0,MaxCount),0),1),"")</f>
         <v/>
       </c>
-      <c r="D50" s="17" t="s">
+      <c r="D50" s="16" t="s">
         <v>110</v>
       </c>
       <c r="E50" s="13" t="str">
@@ -2308,17 +2289,6 @@
       <c r="H50" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="I50" s="18"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="18"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="18"/>
-      <c r="N50" s="18"/>
-      <c r="O50" s="18"/>
-      <c r="P50" s="18"/>
-      <c r="Q50" s="18"/>
-      <c r="R50" s="18"/>
-      <c r="S50" s="18"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
@@ -21905,10 +21875,10 @@
   <sheetFormatPr defaultColWidth="8.64453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="20" t="n">
+      <c r="B1" s="18" t="n">
         <v>2000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat：update new dragon girl icon
</commit_message>
<xml_diff>
--- a/dragon-verse/Excels/BagItem_背包物品表.xlsx
+++ b/dragon-verse/Excels/BagItem_背包物品表.xlsx
@@ -785,8 +785,8 @@
   </sheetPr>
   <dimension ref="A1:N2000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E47" activeCellId="0" sqref="E47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D58" activeCellId="0" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8828125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1074,7 +1074,7 @@
         <v/>
       </c>
       <c r="F10" s="13" t="n">
-        <v>381551</v>
+        <v>388645</v>
       </c>
       <c r="G10" s="13" t="n">
         <v>1</v>
@@ -1105,7 +1105,7 @@
         <v/>
       </c>
       <c r="F11" s="13" t="n">
-        <v>381547</v>
+        <v>388647</v>
       </c>
       <c r="G11" s="13" t="n">
         <v>1</v>
@@ -1199,7 +1199,7 @@
         <v/>
       </c>
       <c r="F14" s="13" t="n">
-        <v>381596</v>
+        <v>388638</v>
       </c>
       <c r="G14" s="13" t="n">
         <v>1</v>
@@ -1397,7 +1397,7 @@
         <v/>
       </c>
       <c r="F20" s="13" t="n">
-        <v>381549</v>
+        <v>388644</v>
       </c>
       <c r="G20" s="13" t="n">
         <v>1</v>
@@ -1460,7 +1460,7 @@
         <v/>
       </c>
       <c r="F22" s="13" t="n">
-        <v>326244</v>
+        <v>388636</v>
       </c>
       <c r="G22" s="13" t="n">
         <v>1</v>
@@ -1520,7 +1520,7 @@
         <v/>
       </c>
       <c r="F24" s="13" t="n">
-        <v>381550</v>
+        <v>388639</v>
       </c>
       <c r="G24" s="13" t="n">
         <v>1</v>
@@ -1760,7 +1760,7 @@
         <v/>
       </c>
       <c r="F32" s="13" t="n">
-        <v>381552</v>
+        <v>388641</v>
       </c>
       <c r="G32" s="13" t="n">
         <v>1</v>
@@ -1790,7 +1790,7 @@
         <v/>
       </c>
       <c r="F33" s="13" t="n">
-        <v>381602</v>
+        <v>388635</v>
       </c>
       <c r="G33" s="13" t="n">
         <v>1</v>
@@ -1880,7 +1880,7 @@
         <v/>
       </c>
       <c r="F36" s="13" t="n">
-        <v>381600</v>
+        <v>388640</v>
       </c>
       <c r="G36" s="13" t="n">
         <v>1</v>
@@ -2253,7 +2253,7 @@
         <v/>
       </c>
       <c r="F49" s="13" t="n">
-        <v>386905</v>
+        <v>388643</v>
       </c>
       <c r="G49" s="13" t="n">
         <v>1</v>
@@ -2281,7 +2281,7 @@
         <v/>
       </c>
       <c r="F50" s="13" t="n">
-        <v>381597</v>
+        <v>388646</v>
       </c>
       <c r="G50" s="13" t="n">
         <v>1</v>

</xml_diff>